<commit_message>
Fixed inclusion of errors from Chen, thorough comparison to fncross, and additional errors detected
+ The pseudo-magnetic parameters from the corrections pointed out by Chen don't need to be rescaled as in our case. Fixing this has substantially improved the reproduction of the data for neodymium in LaF3.
+ The notebook "Table Comparisons.nb" has a thorough comparison of the reduced matrix elements contained in corrected and defective fncross files. This notebook also contains the code necessary to parse the data contained in the fncross files. This analysis resulted in the identification of additional errors in the defective fncross files that were not fixed by Chen. These errors are in the reduced matrix elements for the three body operators.
+ The folder /data/fncrosswhite_old contains defective fncross files. This data has been parsed into a Mathematica association saved as /data/fncross_old.m. The parsed corrected version /data/fncross.m has been updated with improved parsing.
</commit_message>
<xml_diff>
--- a/data/Carnall - 1968 - Table 1.xlsx
+++ b/data/Carnall - 1968 - Table 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/ZiaLab/Codebase/qlanth/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA9C730-F649-3E4E-A8AB-9217172E4777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867DF224-3BB4-2546-ADB9-74720FDBA36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="17280" windowHeight="21700" xr2:uid="{01874963-C738-B449-9CDD-5BD4FE2B6E37}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="21600" xr2:uid="{01874963-C738-B449-9CDD-5BD4FE2B6E37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -331,9 +331,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -371,7 +371,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -477,7 +477,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -619,7 +619,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -630,7 +630,7 @@
   <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="192" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -713,7 +713,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>

</xml_diff>